<commit_message>
Corrige mapeo de campo RFC para F63
</commit_message>
<xml_diff>
--- a/Forma 63 to db.xlsx
+++ b/Forma 63 to db.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joreyes\Desktop\archivos_integracion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4759EE5-8013-4EA8-A791-EB44361AE5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B39F95A3-59AA-448C-83E5-E8176CD2693D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="5" xr2:uid="{E20FB620-34D1-4B11-8D20-35239AC56F26}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="1" activeTab="1" xr2:uid="{E20FB620-34D1-4B11-8D20-35239AC56F26}"/>
   </bookViews>
   <sheets>
     <sheet name="TablasUnicas" sheetId="3" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7198" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7198" uniqueCount="808">
   <si>
     <t>Nombre de la Entidad</t>
   </si>
@@ -2442,9 +2442,6 @@
     <t>MM_DEC_CDIRFPA1.N_DEC_EDFJOIE1</t>
   </si>
   <si>
-    <t>MM_DEC_CDIRFPA1.D_DEC_RFCEEEO1</t>
-  </si>
-  <si>
     <t>MM_DEC_CDIRFPA1.C_IDC_ICDOENN1</t>
   </si>
   <si>
@@ -2460,9 +2457,6 @@
     <t>Restricciones</t>
   </si>
   <si>
-    <t>NOT NULL PRIMARY KEY</t>
-  </si>
-  <si>
     <t>Tipo de dato (db)</t>
   </si>
   <si>
@@ -2482,6 +2476,15 @@
   </si>
   <si>
     <t>Nombre del atributo</t>
+  </si>
+  <si>
+    <t>FK</t>
+  </si>
+  <si>
+    <t>PK</t>
+  </si>
+  <si>
+    <t>MM_DEC_CDIRFPA1.D_DEC_RFCEDDE1</t>
   </si>
 </sst>
 </file>
@@ -3084,7 +3087,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3197,6 +3200,12 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -3698,8 +3707,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K190"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:D1048576"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.5" x14ac:dyDescent="0.25"/>
@@ -4294,19 +4303,19 @@
         <v>544</v>
       </c>
       <c r="C1" s="8" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="D1" s="8" t="s">
         <v>548</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="F1" s="8" t="s">
         <v>181</v>
       </c>
       <c r="G1" s="8" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>181</v>
@@ -7156,7 +7165,7 @@
         <v>182</v>
       </c>
       <c r="G87" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="H87" s="2" t="s">
         <v>183</v>
@@ -10554,8 +10563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85DC6DC5-7EE4-4BE3-9327-077902235360}">
   <dimension ref="A1:BF178"/>
   <sheetViews>
-    <sheetView topLeftCell="A143" workbookViewId="0">
-      <selection activeCell="C157" sqref="C157"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D90" sqref="D90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -11763,7 +11772,7 @@
       <c r="C95" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="D95" s="2"/>
+      <c r="D95" s="43"/>
     </row>
     <row r="96" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2" t="s">
@@ -11775,7 +11784,7 @@
       <c r="C96" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D96" s="2" t="s">
+      <c r="D96" s="43" t="s">
         <v>792</v>
       </c>
       <c r="E96"/>
@@ -11843,8 +11852,8 @@
       <c r="C97" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D97" s="9" t="s">
-        <v>794</v>
+      <c r="D97" s="43" t="s">
+        <v>793</v>
       </c>
       <c r="E97"/>
       <c r="F97"/>
@@ -11911,8 +11920,8 @@
       <c r="C98" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>793</v>
+      <c r="D98" s="43" t="s">
+        <v>807</v>
       </c>
       <c r="E98"/>
       <c r="F98"/>
@@ -11979,8 +11988,8 @@
       <c r="C99" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="D99" s="20" t="s">
-        <v>795</v>
+      <c r="D99" s="44" t="s">
+        <v>794</v>
       </c>
       <c r="E99"/>
       <c r="F99"/>
@@ -12047,7 +12056,7 @@
       <c r="C100" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="D100" s="2"/>
+      <c r="D100" s="43"/>
     </row>
     <row r="101" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A101" s="2" t="s">
@@ -12059,7 +12068,7 @@
       <c r="C101" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="D101" s="2"/>
+      <c r="D101" s="43"/>
     </row>
     <row r="102" spans="1:58" x14ac:dyDescent="0.35">
       <c r="A102" s="2" t="s">
@@ -13010,7 +13019,7 @@
         <v>79</v>
       </c>
       <c r="D171" s="9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="E171"/>
       <c r="F171"/>
@@ -13076,8 +13085,8 @@
       <c r="C172" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D172" s="9" t="s">
-        <v>793</v>
+      <c r="D172" s="43" t="s">
+        <v>807</v>
       </c>
       <c r="E172"/>
       <c r="F172"/>
@@ -13144,7 +13153,7 @@
         <v>65</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="E173"/>
       <c r="F173"/>
@@ -13265,6 +13274,7 @@
     <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -13272,8 +13282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAE4105-2D27-41A8-97C1-D84AE1DB6648}">
   <dimension ref="A1:F190"/>
   <sheetViews>
-    <sheetView topLeftCell="A147" workbookViewId="0">
-      <selection activeCell="C161" sqref="C161"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F178" sqref="F178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -13296,13 +13306,13 @@
         <v>548</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>795</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>796</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>797</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>798</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -13322,7 +13332,7 @@
         <v>190</v>
       </c>
       <c r="F2" s="15" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -14851,7 +14861,7 @@
         <v>184</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="F87" s="2"/>
     </row>
@@ -15050,7 +15060,7 @@
         <v>190</v>
       </c>
       <c r="F98" s="15" t="s">
-        <v>799</v>
+        <v>805</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.35">
@@ -15070,7 +15080,7 @@
         <v>211</v>
       </c>
       <c r="F99" s="15" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.35">
@@ -16438,7 +16448,7 @@
         <v>190</v>
       </c>
       <c r="F175" s="15" t="s">
-        <v>799</v>
+        <v>805</v>
       </c>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.35">
@@ -16476,7 +16486,7 @@
         <v>211</v>
       </c>
       <c r="F177" s="15" t="s">
-        <v>799</v>
+        <v>806</v>
       </c>
     </row>
     <row r="178" spans="1:6" x14ac:dyDescent="0.35">
@@ -20114,7 +20124,7 @@
       </c>
       <c r="N77" s="7"/>
       <c r="O77" s="33" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="P77" s="7" t="s">
         <v>649</v>
@@ -20161,7 +20171,7 @@
       <c r="M78" s="5"/>
       <c r="N78" s="5"/>
       <c r="O78" s="33" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="P78" s="7" t="s">
         <v>650</v>
@@ -20206,7 +20216,7 @@
       <c r="M79" s="5"/>
       <c r="N79" s="5"/>
       <c r="O79" s="33" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="P79" s="7" t="s">
         <v>651</v>
@@ -24233,7 +24243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1813603-804A-49E6-BE96-FC408FACBFE5}">
   <dimension ref="A1:C190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A23" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -24249,7 +24259,7 @@
         <v>544</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>548</v>
@@ -24310,7 +24320,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" ht="24" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>78</v>
       </c>
@@ -24321,7 +24331,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" ht="24" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>78</v>
       </c>
@@ -24816,7 +24826,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="24" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A53" s="2" t="s">
         <v>78</v>
       </c>
@@ -25025,7 +25035,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:3" ht="24" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A72" s="2" t="s">
         <v>78</v>
       </c>
@@ -25091,7 +25101,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="24" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A78" s="2" t="s">
         <v>78</v>
       </c>
@@ -25586,7 +25596,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A123" s="2" t="s">
         <v>102</v>
       </c>
@@ -25608,7 +25618,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="125" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A125" s="2" t="s">
         <v>102</v>
       </c>
@@ -25630,7 +25640,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A127" s="2" t="s">
         <v>102</v>
       </c>
@@ -25652,7 +25662,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A129" s="2" t="s">
         <v>102</v>
       </c>
@@ -25674,7 +25684,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A131" s="2" t="s">
         <v>102</v>
       </c>
@@ -25696,7 +25706,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="133" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A133" s="2" t="s">
         <v>102</v>
       </c>
@@ -25707,7 +25717,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="134" spans="1:3" ht="58.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:3" ht="47" x14ac:dyDescent="0.35">
       <c r="A134" s="2" t="s">
         <v>102</v>
       </c>
@@ -25718,7 +25728,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A135" s="2" t="s">
         <v>102</v>
       </c>
@@ -25740,7 +25750,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A137" s="2" t="s">
         <v>102</v>
       </c>
@@ -25762,7 +25772,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="139" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A139" s="2" t="s">
         <v>102</v>
       </c>
@@ -25784,7 +25794,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A141" s="2" t="s">
         <v>102</v>
       </c>
@@ -25806,7 +25816,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="143" spans="1:3" ht="70" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:3" ht="58.5" x14ac:dyDescent="0.35">
       <c r="A143" s="2" t="s">
         <v>102</v>
       </c>
@@ -25817,7 +25827,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="144" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A144" s="2" t="s">
         <v>102</v>
       </c>
@@ -25828,7 +25838,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="81.5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:3" ht="70" x14ac:dyDescent="0.35">
       <c r="A145" s="2" t="s">
         <v>102</v>
       </c>
@@ -25894,7 +25904,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="70" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:3" ht="58.5" x14ac:dyDescent="0.35">
       <c r="A151" s="2" t="s">
         <v>102</v>
       </c>
@@ -26081,7 +26091,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="168" spans="1:3" ht="35.5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:3" ht="24" x14ac:dyDescent="0.35">
       <c r="A168" s="2" t="s">
         <v>102</v>
       </c>
@@ -26092,7 +26102,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="47" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:3" ht="35.5" x14ac:dyDescent="0.35">
       <c r="A169" s="2" t="s">
         <v>102</v>
       </c>
@@ -26415,7 +26425,7 @@
         <v>558</v>
       </c>
       <c r="P1" s="8" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="Q1" s="8" t="s">
         <v>559</v>
@@ -31414,7 +31424,7 @@
       <c r="M111" s="5"/>
       <c r="N111" s="5"/>
       <c r="O111" s="12" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="P111" s="12"/>
       <c r="Q111" s="5" t="s">

</xml_diff>